<commit_message>
model updates - added adult model
</commit_message>
<xml_diff>
--- a/parameters/inp_par_dmc.xlsx
+++ b/parameters/inp_par_dmc.xlsx
@@ -2,19 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcoomes/Dropbox/HIV modeling/HIV-syphilis-hbv model/parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcoomes/repos/hiv_syphilis_hbv_model/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F3614C-D6AC-E14D-B000-EFB4A62FBFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE97D0C-E980-9E4E-8861-5C2A3921BE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="760" windowWidth="27640" windowHeight="16940" xr2:uid="{754DE57E-8490-E64C-A72A-B0E2176D4FB0}"/>
+    <workbookView xWindow="1780" yWindow="760" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{754DE57E-8490-E64C-A72A-B0E2176D4FB0}"/>
   </bookViews>
   <sheets>
     <sheet name="pop_characteristics" sheetId="1" r:id="rId1"/>
     <sheet name="test_characteristics" sheetId="2" r:id="rId2"/>
+    <sheet name="adult_model_characteristics" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1685" uniqueCount="430">
   <si>
     <t>model</t>
   </si>
@@ -1240,13 +1241,100 @@
   </si>
   <si>
     <t>rdt_sens_hiv_a</t>
+  </si>
+  <si>
+    <t>Annual syphilis testing rate for non-pregnant women</t>
+  </si>
+  <si>
+    <t>syph_test_prob</t>
+  </si>
+  <si>
+    <t>hiv_inc</t>
+  </si>
+  <si>
+    <t>UNAIDS</t>
+  </si>
+  <si>
+    <t>https://www.unaids.org/en/regionscountries/countries/kenya</t>
+  </si>
+  <si>
+    <t>Annual HIV incidence rate (adults aged 15-49)</t>
+  </si>
+  <si>
+    <t>Annual HIV incidence rate (women aged 15-49)</t>
+  </si>
+  <si>
+    <t>hiv_inc_female</t>
+  </si>
+  <si>
+    <t>Annual HIV incidence rate (men aged 15-49)</t>
+  </si>
+  <si>
+    <t>hiv_inc_male</t>
+  </si>
+  <si>
+    <t>Calculated as weighted average of male and female incident infections on incidence rate</t>
+  </si>
+  <si>
+    <t>pct_ART</t>
+  </si>
+  <si>
+    <t>supp_vl</t>
+  </si>
+  <si>
+    <t>% of PLWH on ART</t>
+  </si>
+  <si>
+    <t>% of PLWH virally suppressed</t>
+  </si>
+  <si>
+    <t>% of women living with HIV on ART</t>
+  </si>
+  <si>
+    <t>pct_ART_female</t>
+  </si>
+  <si>
+    <t>Adult screening rate</t>
+  </si>
+  <si>
+    <t>adult_screen_hiv</t>
+  </si>
+  <si>
+    <t>Maternal model</t>
+  </si>
+  <si>
+    <t>General population model</t>
+  </si>
+  <si>
+    <t>HIV_Syphilis_Dual</t>
+  </si>
+  <si>
+    <t>adult_pop</t>
+  </si>
+  <si>
+    <t>Adult population (adults aged 15-64)</t>
+  </si>
+  <si>
+    <t>HIV prevalence</t>
+  </si>
+  <si>
+    <t>hiv_prev_adult</t>
+  </si>
+  <si>
+    <t>HIV incidence reduction due to ART use</t>
+  </si>
+  <si>
+    <t>https://pmc.ncbi.nlm.nih.gov/articles/PMC5049503/</t>
+  </si>
+  <si>
+    <t>hiv_red_ART</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1383,6 +1471,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1697,7 +1793,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1740,8 +1836,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1749,8 +1846,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1784,6 +1882,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2124,10 +2223,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E74D272-9445-3049-81AC-6093333D4DBD}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="H190" sqref="H190"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D159" sqref="D159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5530,6 +5630,9 @@
       <c r="E115" t="s">
         <v>48</v>
       </c>
+      <c r="F115" t="s">
+        <v>49</v>
+      </c>
       <c r="G115">
         <v>4.4000000000000003E-3</v>
       </c>
@@ -8109,10 +8212,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9493A486-73AE-4849-B9D6-E454460A1CA7}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8766,4 +8870,377 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D20474-A433-3B45-BD81-C94AF5EBE7BE}">
+  <dimension ref="A1:M12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="52.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>420</v>
+      </c>
+      <c r="E2" t="s">
+        <v>401</v>
+      </c>
+      <c r="F2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>328</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>420</v>
+      </c>
+      <c r="E3" t="s">
+        <v>406</v>
+      </c>
+      <c r="F3" t="s">
+        <v>403</v>
+      </c>
+      <c r="G3">
+        <f>0.53/1000</f>
+        <v>5.2999999999999998E-4</v>
+      </c>
+      <c r="H3">
+        <v>3.2000000000000003E-4</v>
+      </c>
+      <c r="I3">
+        <v>8.3000000000000001E-4</v>
+      </c>
+      <c r="J3">
+        <v>2024</v>
+      </c>
+      <c r="K3" t="s">
+        <v>404</v>
+      </c>
+      <c r="L3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>328</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E4" t="s">
+        <v>407</v>
+      </c>
+      <c r="F4" t="s">
+        <v>408</v>
+      </c>
+      <c r="G4">
+        <f>0.00053 * (11000 / (11000+4600)) * 2</f>
+        <v>7.4743589743589748E-4</v>
+      </c>
+      <c r="J4">
+        <v>2024</v>
+      </c>
+      <c r="K4" t="s">
+        <v>404</v>
+      </c>
+      <c r="L4" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>420</v>
+      </c>
+      <c r="E5" t="s">
+        <v>409</v>
+      </c>
+      <c r="F5" t="s">
+        <v>410</v>
+      </c>
+      <c r="G5">
+        <f>0.00053 * (4600 / (11000+4600)) * 2</f>
+        <v>3.1256410256410254E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>328</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>420</v>
+      </c>
+      <c r="E6" t="s">
+        <v>414</v>
+      </c>
+      <c r="F6" t="s">
+        <v>412</v>
+      </c>
+      <c r="G6">
+        <v>0.87</v>
+      </c>
+      <c r="H6">
+        <v>0.78</v>
+      </c>
+      <c r="I6">
+        <v>0.97</v>
+      </c>
+      <c r="J6">
+        <v>2024</v>
+      </c>
+      <c r="K6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>420</v>
+      </c>
+      <c r="E7" t="s">
+        <v>416</v>
+      </c>
+      <c r="F7" t="s">
+        <v>417</v>
+      </c>
+      <c r="G7">
+        <v>0.9</v>
+      </c>
+      <c r="H7">
+        <v>0.8</v>
+      </c>
+      <c r="I7">
+        <v>0.98</v>
+      </c>
+      <c r="J7">
+        <v>2024</v>
+      </c>
+      <c r="K7" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>328</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>420</v>
+      </c>
+      <c r="E8" t="s">
+        <v>415</v>
+      </c>
+      <c r="F8" t="s">
+        <v>413</v>
+      </c>
+      <c r="G8">
+        <v>0.83</v>
+      </c>
+      <c r="H8">
+        <v>0.74</v>
+      </c>
+      <c r="I8">
+        <v>0.95</v>
+      </c>
+      <c r="J8">
+        <v>2024</v>
+      </c>
+      <c r="K8" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>328</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>420</v>
+      </c>
+      <c r="E9" t="s">
+        <v>418</v>
+      </c>
+      <c r="F9" t="s">
+        <v>419</v>
+      </c>
+      <c r="G9">
+        <v>0.8</v>
+      </c>
+      <c r="K9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>422</v>
+      </c>
+      <c r="B10" t="s">
+        <v>328</v>
+      </c>
+      <c r="C10" t="s">
+        <v>330</v>
+      </c>
+      <c r="D10" t="s">
+        <v>421</v>
+      </c>
+      <c r="E10" t="s">
+        <v>424</v>
+      </c>
+      <c r="F10" t="s">
+        <v>423</v>
+      </c>
+      <c r="G10">
+        <v>33971376</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>328</v>
+      </c>
+      <c r="D11" t="s">
+        <v>421</v>
+      </c>
+      <c r="E11" t="s">
+        <v>425</v>
+      </c>
+      <c r="F11" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>421</v>
+      </c>
+      <c r="E12" t="s">
+        <v>427</v>
+      </c>
+      <c r="F12" t="s">
+        <v>429</v>
+      </c>
+      <c r="G12">
+        <v>0.93</v>
+      </c>
+      <c r="H12">
+        <v>0.78</v>
+      </c>
+      <c r="I12">
+        <v>0.98</v>
+      </c>
+      <c r="J12">
+        <v>2016</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K12" r:id="rId1" xr:uid="{DC91DADF-43FA-B041-95AE-EE9D543D2F82}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>